<commit_message>
New version of the sex vocabolary where metadata URIs have been fixed, the publisheer and creator have been changed according to schema.gov.it governance and semantic alignments with the human sex Publications Office's EU vocabulary have been created. In addition, the csv and xlsx version of the vocabulary meet the requests in issues #170
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-people/sex/sex.xlsx
+++ b/VocabolariControllati/classifications-for-people/sex/sex.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-people/sex/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E6936-FC47-2B40-B47A-3916A51DEC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,16 +48,16 @@
     <t>codice_1 _Llivello</t>
   </si>
   <si>
-    <t>label_ITA_1_livello</t>
-  </si>
-  <si>
-    <t>label_ENG_1_livello</t>
+    <t>label_1_livello_it</t>
+  </si>
+  <si>
+    <t>label_1_livello_en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,16 +126,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -454,21 +468,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -479,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -490,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
New version of the sex vocabolary where metadata URIs have been fixed, the publisheer and creator have been changed according to schema.gov.it governance and semantic alignments with the human sex Publications Office's EU vocabulary have been created. In addition, the csv and xlsx version of the vocabulary meet the requests in issues #170 (#207)
Co-authored-by: Giorgia Lodi <giorgialodi@Giorgias-MacBook-Pro.local>
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-people/sex/sex.xlsx
+++ b/VocabolariControllati/classifications-for-people/sex/sex.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-people/sex/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E6936-FC47-2B40-B47A-3916A51DEC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,16 +48,16 @@
     <t>codice_1 _Llivello</t>
   </si>
   <si>
-    <t>label_ITA_1_livello</t>
-  </si>
-  <si>
-    <t>label_ENG_1_livello</t>
+    <t>label_1_livello_it</t>
+  </si>
+  <si>
+    <t>label_1_livello_en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,16 +126,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -454,21 +468,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -479,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -490,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>